<commit_message>
calculator: major refactoring, inspection draft
</commit_message>
<xml_diff>
--- a/public/local/fixtures/calculator/Обследование калькуляторы.xlsx
+++ b/public/local/fixtures/calculator/Обследование калькуляторы.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37520" windowHeight="21140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37580" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Обследование одного здания" sheetId="3" r:id="rId1"/>
@@ -400,9 +400,6 @@
     <t>более 100 000 кв.м.</t>
   </si>
   <si>
-    <t>30 раб дн.</t>
-  </si>
-  <si>
     <t>35 раб. дн.</t>
   </si>
   <si>
@@ -740,6 +737,9 @@
   </si>
   <si>
     <t>11. Цели обследования*</t>
+  </si>
+  <si>
+    <t>30 раб. дн.</t>
   </si>
 </sst>
 </file>
@@ -1364,7 +1364,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1408,6 +1408,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1528,9 +1532,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1538,8 +1539,11 @@
     </xf>
     <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="71">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1581,6 +1585,8 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1598,6 +1604,8 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1886,13 +1894,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="F171" sqref="F171"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="D251" sqref="D251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="39"/>
+    <col min="1" max="1" width="8.83203125" style="38"/>
     <col min="2" max="2" width="53.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" style="16" customWidth="1"/>
@@ -1918,7 +1926,7 @@
     </row>
     <row r="4" spans="1:32" ht="15">
       <c r="B4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="15"/>
     </row>
@@ -1928,12 +1936,12 @@
     </row>
     <row r="6" spans="1:32" ht="14.25" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="39">
+      <c r="A7" s="38">
         <v>1</v>
       </c>
       <c r="B7" s="3">
@@ -1944,7 +1952,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A8" s="39"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="2"/>
       <c r="C8" s="15"/>
       <c r="AD8" s="13"/>
@@ -1952,9 +1960,9 @@
       <c r="AF8" s="13"/>
     </row>
     <row r="9" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A9" s="39"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="15"/>
       <c r="AD9" s="13"/>
@@ -1962,7 +1970,7 @@
       <c r="AF9" s="13"/>
     </row>
     <row r="10" spans="1:32" s="16" customFormat="1">
-      <c r="A10" s="39">
+      <c r="A10" s="38">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1976,7 +1984,7 @@
       <c r="AF10" s="13"/>
     </row>
     <row r="11" spans="1:32" s="16" customFormat="1">
-      <c r="A11" s="39">
+      <c r="A11" s="38">
         <v>2</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1990,7 +1998,7 @@
       <c r="AF11" s="13"/>
     </row>
     <row r="12" spans="1:32" s="16" customFormat="1">
-      <c r="A12" s="39">
+      <c r="A12" s="38">
         <v>3</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2004,7 +2012,7 @@
       <c r="AF12" s="13"/>
     </row>
     <row r="13" spans="1:32" s="16" customFormat="1">
-      <c r="A13" s="39">
+      <c r="A13" s="38">
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2018,7 +2026,7 @@
       <c r="AF13" s="13"/>
     </row>
     <row r="14" spans="1:32" s="16" customFormat="1">
-      <c r="A14" s="39">
+      <c r="A14" s="38">
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2032,7 +2040,7 @@
       <c r="AF14" s="13"/>
     </row>
     <row r="15" spans="1:32" s="16" customFormat="1">
-      <c r="A15" s="39">
+      <c r="A15" s="38">
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2046,7 +2054,7 @@
       <c r="AF15" s="13"/>
     </row>
     <row r="16" spans="1:32" s="16" customFormat="1">
-      <c r="A16" s="39">
+      <c r="A16" s="38">
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2060,7 +2068,7 @@
       <c r="AF16" s="13"/>
     </row>
     <row r="17" spans="1:32" s="16" customFormat="1">
-      <c r="A17" s="39">
+      <c r="A17" s="38">
         <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -2074,7 +2082,7 @@
       <c r="AF17" s="13"/>
     </row>
     <row r="18" spans="1:32" s="16" customFormat="1">
-      <c r="A18" s="39">
+      <c r="A18" s="38">
         <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -2088,7 +2096,7 @@
       <c r="AF18" s="13"/>
     </row>
     <row r="19" spans="1:32" s="16" customFormat="1">
-      <c r="A19" s="39">
+      <c r="A19" s="38">
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -2102,7 +2110,7 @@
       <c r="AF19" s="13"/>
     </row>
     <row r="20" spans="1:32" s="16" customFormat="1">
-      <c r="A20" s="39">
+      <c r="A20" s="38">
         <v>11</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2116,7 +2124,7 @@
       <c r="AF20" s="13"/>
     </row>
     <row r="21" spans="1:32" s="16" customFormat="1">
-      <c r="A21" s="39">
+      <c r="A21" s="38">
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -2130,7 +2138,7 @@
       <c r="AF21" s="13"/>
     </row>
     <row r="22" spans="1:32" s="16" customFormat="1">
-      <c r="A22" s="39">
+      <c r="A22" s="38">
         <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -2144,7 +2152,7 @@
       <c r="AF22" s="13"/>
     </row>
     <row r="23" spans="1:32" s="16" customFormat="1">
-      <c r="A23" s="39">
+      <c r="A23" s="38">
         <v>14</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2158,7 +2166,7 @@
       <c r="AF23" s="13"/>
     </row>
     <row r="24" spans="1:32" s="16" customFormat="1">
-      <c r="A24" s="39">
+      <c r="A24" s="38">
         <v>15</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2172,7 +2180,7 @@
       <c r="AF24" s="13"/>
     </row>
     <row r="25" spans="1:32" s="16" customFormat="1">
-      <c r="A25" s="39">
+      <c r="A25" s="38">
         <v>16</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2186,7 +2194,7 @@
       <c r="AF25" s="13"/>
     </row>
     <row r="26" spans="1:32" s="16" customFormat="1">
-      <c r="A26" s="39">
+      <c r="A26" s="38">
         <v>17</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -2200,7 +2208,7 @@
       <c r="AF26" s="13"/>
     </row>
     <row r="27" spans="1:32" s="16" customFormat="1">
-      <c r="A27" s="39">
+      <c r="A27" s="38">
         <v>18</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -2214,7 +2222,7 @@
       <c r="AF27" s="13"/>
     </row>
     <row r="28" spans="1:32" s="16" customFormat="1">
-      <c r="A28" s="39">
+      <c r="A28" s="38">
         <v>19</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -2228,7 +2236,7 @@
       <c r="AF28" s="13"/>
     </row>
     <row r="29" spans="1:32" s="16" customFormat="1">
-      <c r="A29" s="39">
+      <c r="A29" s="38">
         <v>20</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -2242,7 +2250,7 @@
       <c r="AF29" s="13"/>
     </row>
     <row r="30" spans="1:32" s="16" customFormat="1">
-      <c r="A30" s="39">
+      <c r="A30" s="38">
         <v>21</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -2256,7 +2264,7 @@
       <c r="AF30" s="13"/>
     </row>
     <row r="31" spans="1:32" s="16" customFormat="1">
-      <c r="A31" s="39">
+      <c r="A31" s="38">
         <v>22</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -2270,7 +2278,7 @@
       <c r="AF31" s="13"/>
     </row>
     <row r="32" spans="1:32" s="16" customFormat="1">
-      <c r="A32" s="39">
+      <c r="A32" s="38">
         <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -2284,7 +2292,7 @@
       <c r="AF32" s="13"/>
     </row>
     <row r="33" spans="1:32" s="16" customFormat="1">
-      <c r="A33" s="39">
+      <c r="A33" s="38">
         <v>24</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -2298,7 +2306,7 @@
       <c r="AF33" s="13"/>
     </row>
     <row r="34" spans="1:32" s="16" customFormat="1">
-      <c r="A34" s="39">
+      <c r="A34" s="38">
         <v>25</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -2312,7 +2320,7 @@
       <c r="AF34" s="13"/>
     </row>
     <row r="35" spans="1:32" s="16" customFormat="1">
-      <c r="A35" s="39">
+      <c r="A35" s="38">
         <v>26</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -2326,7 +2334,7 @@
       <c r="AF35" s="13"/>
     </row>
     <row r="36" spans="1:32" s="16" customFormat="1">
-      <c r="A36" s="39">
+      <c r="A36" s="38">
         <v>27</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -2340,7 +2348,7 @@
       <c r="AF36" s="13"/>
     </row>
     <row r="37" spans="1:32" s="16" customFormat="1">
-      <c r="A37" s="39">
+      <c r="A37" s="38">
         <v>28</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -2354,7 +2362,7 @@
       <c r="AF37" s="13"/>
     </row>
     <row r="38" spans="1:32" s="16" customFormat="1">
-      <c r="A38" s="39">
+      <c r="A38" s="38">
         <v>29</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -2368,7 +2376,7 @@
       <c r="AF38" s="13"/>
     </row>
     <row r="39" spans="1:32" s="16" customFormat="1">
-      <c r="A39" s="39">
+      <c r="A39" s="38">
         <v>30</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -2382,7 +2390,7 @@
       <c r="AF39" s="13"/>
     </row>
     <row r="40" spans="1:32" s="16" customFormat="1">
-      <c r="A40" s="39">
+      <c r="A40" s="38">
         <v>31</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -2396,7 +2404,7 @@
       <c r="AF40" s="13"/>
     </row>
     <row r="41" spans="1:32" s="16" customFormat="1">
-      <c r="A41" s="39">
+      <c r="A41" s="38">
         <v>32</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -2410,7 +2418,7 @@
       <c r="AF41" s="13"/>
     </row>
     <row r="42" spans="1:32" s="16" customFormat="1">
-      <c r="A42" s="39">
+      <c r="A42" s="38">
         <v>33</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -2424,7 +2432,7 @@
       <c r="AF42" s="13"/>
     </row>
     <row r="43" spans="1:32" s="16" customFormat="1">
-      <c r="A43" s="39">
+      <c r="A43" s="38">
         <v>34</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -2438,7 +2446,7 @@
       <c r="AF43" s="13"/>
     </row>
     <row r="44" spans="1:32" s="16" customFormat="1">
-      <c r="A44" s="39">
+      <c r="A44" s="38">
         <v>35</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -2452,7 +2460,7 @@
       <c r="AF44" s="13"/>
     </row>
     <row r="45" spans="1:32" s="16" customFormat="1">
-      <c r="A45" s="39">
+      <c r="A45" s="38">
         <v>36</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -2466,7 +2474,7 @@
       <c r="AF45" s="13"/>
     </row>
     <row r="46" spans="1:32" s="16" customFormat="1">
-      <c r="A46" s="39">
+      <c r="A46" s="38">
         <v>37</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -2480,7 +2488,7 @@
       <c r="AF46" s="13"/>
     </row>
     <row r="47" spans="1:32" s="16" customFormat="1">
-      <c r="A47" s="39">
+      <c r="A47" s="38">
         <v>38</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -2494,7 +2502,7 @@
       <c r="AF47" s="13"/>
     </row>
     <row r="48" spans="1:32" s="16" customFormat="1">
-      <c r="A48" s="39">
+      <c r="A48" s="38">
         <v>39</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -2508,7 +2516,7 @@
       <c r="AF48" s="13"/>
     </row>
     <row r="49" spans="1:32" s="16" customFormat="1">
-      <c r="A49" s="39">
+      <c r="A49" s="38">
         <v>40</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -2522,7 +2530,7 @@
       <c r="AF49" s="13"/>
     </row>
     <row r="50" spans="1:32" s="16" customFormat="1">
-      <c r="A50" s="39">
+      <c r="A50" s="38">
         <v>41</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -2536,7 +2544,7 @@
       <c r="AF50" s="13"/>
     </row>
     <row r="51" spans="1:32" s="16" customFormat="1">
-      <c r="A51" s="39">
+      <c r="A51" s="38">
         <v>42</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -2550,7 +2558,7 @@
       <c r="AF51" s="13"/>
     </row>
     <row r="52" spans="1:32" s="16" customFormat="1">
-      <c r="A52" s="39">
+      <c r="A52" s="38">
         <v>43</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -2564,7 +2572,7 @@
       <c r="AF52" s="13"/>
     </row>
     <row r="53" spans="1:32" s="16" customFormat="1">
-      <c r="A53" s="39">
+      <c r="A53" s="38">
         <v>44</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -2578,7 +2586,7 @@
       <c r="AF53" s="13"/>
     </row>
     <row r="54" spans="1:32" s="16" customFormat="1">
-      <c r="A54" s="39">
+      <c r="A54" s="38">
         <v>45</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -2592,7 +2600,7 @@
       <c r="AF54" s="13"/>
     </row>
     <row r="55" spans="1:32" s="16" customFormat="1">
-      <c r="A55" s="39">
+      <c r="A55" s="38">
         <v>46</v>
       </c>
       <c r="B55" s="4" t="s">
@@ -2606,7 +2614,7 @@
       <c r="AF55" s="13"/>
     </row>
     <row r="56" spans="1:32" s="16" customFormat="1">
-      <c r="A56" s="39">
+      <c r="A56" s="38">
         <v>47</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -2620,7 +2628,7 @@
       <c r="AF56" s="13"/>
     </row>
     <row r="57" spans="1:32" s="16" customFormat="1">
-      <c r="A57" s="39">
+      <c r="A57" s="38">
         <v>48</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -2634,7 +2642,7 @@
       <c r="AF57" s="13"/>
     </row>
     <row r="58" spans="1:32" s="16" customFormat="1">
-      <c r="A58" s="39">
+      <c r="A58" s="38">
         <v>49</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -2648,7 +2656,7 @@
       <c r="AF58" s="13"/>
     </row>
     <row r="59" spans="1:32" s="16" customFormat="1">
-      <c r="A59" s="39">
+      <c r="A59" s="38">
         <v>50</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -2662,7 +2670,7 @@
       <c r="AF59" s="13"/>
     </row>
     <row r="60" spans="1:32" s="16" customFormat="1">
-      <c r="A60" s="39">
+      <c r="A60" s="38">
         <v>51</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -2676,7 +2684,7 @@
       <c r="AF60" s="13"/>
     </row>
     <row r="61" spans="1:32" s="16" customFormat="1">
-      <c r="A61" s="39">
+      <c r="A61" s="38">
         <v>52</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -2690,7 +2698,7 @@
       <c r="AF61" s="13"/>
     </row>
     <row r="62" spans="1:32" s="16" customFormat="1">
-      <c r="A62" s="39">
+      <c r="A62" s="38">
         <v>53</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -2704,7 +2712,7 @@
       <c r="AF62" s="13"/>
     </row>
     <row r="63" spans="1:32" s="16" customFormat="1">
-      <c r="A63" s="39">
+      <c r="A63" s="38">
         <v>54</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -2718,7 +2726,7 @@
       <c r="AF63" s="13"/>
     </row>
     <row r="64" spans="1:32" s="16" customFormat="1">
-      <c r="A64" s="39">
+      <c r="A64" s="38">
         <v>55</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -2732,7 +2740,7 @@
       <c r="AF64" s="13"/>
     </row>
     <row r="65" spans="1:32" s="16" customFormat="1">
-      <c r="A65" s="39">
+      <c r="A65" s="38">
         <v>56</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -2746,7 +2754,7 @@
       <c r="AF65" s="13"/>
     </row>
     <row r="66" spans="1:32" s="16" customFormat="1">
-      <c r="A66" s="39">
+      <c r="A66" s="38">
         <v>57</v>
       </c>
       <c r="B66" s="4" t="s">
@@ -2760,7 +2768,7 @@
       <c r="AF66" s="13"/>
     </row>
     <row r="67" spans="1:32" s="16" customFormat="1">
-      <c r="A67" s="39">
+      <c r="A67" s="38">
         <v>58</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -2774,7 +2782,7 @@
       <c r="AF67" s="13"/>
     </row>
     <row r="68" spans="1:32" s="16" customFormat="1">
-      <c r="A68" s="39">
+      <c r="A68" s="38">
         <v>59</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -2788,7 +2796,7 @@
       <c r="AF68" s="13"/>
     </row>
     <row r="69" spans="1:32" s="16" customFormat="1">
-      <c r="A69" s="39">
+      <c r="A69" s="38">
         <v>60</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -2802,7 +2810,7 @@
       <c r="AF69" s="13"/>
     </row>
     <row r="70" spans="1:32" s="16" customFormat="1">
-      <c r="A70" s="39">
+      <c r="A70" s="38">
         <v>61</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -2816,7 +2824,7 @@
       <c r="AF70" s="13"/>
     </row>
     <row r="71" spans="1:32" s="16" customFormat="1">
-      <c r="A71" s="39">
+      <c r="A71" s="38">
         <v>62</v>
       </c>
       <c r="B71" s="4" t="s">
@@ -2830,7 +2838,7 @@
       <c r="AF71" s="13"/>
     </row>
     <row r="72" spans="1:32" s="16" customFormat="1">
-      <c r="A72" s="39">
+      <c r="A72" s="38">
         <v>63</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -2844,7 +2852,7 @@
       <c r="AF72" s="13"/>
     </row>
     <row r="73" spans="1:32" s="16" customFormat="1">
-      <c r="A73" s="39">
+      <c r="A73" s="38">
         <v>64</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -2858,7 +2866,7 @@
       <c r="AF73" s="13"/>
     </row>
     <row r="74" spans="1:32" s="16" customFormat="1">
-      <c r="A74" s="39">
+      <c r="A74" s="38">
         <v>65</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -2872,7 +2880,7 @@
       <c r="AF74" s="13"/>
     </row>
     <row r="75" spans="1:32" s="16" customFormat="1">
-      <c r="A75" s="39">
+      <c r="A75" s="38">
         <v>66</v>
       </c>
       <c r="B75" s="4" t="s">
@@ -2886,7 +2894,7 @@
       <c r="AF75" s="13"/>
     </row>
     <row r="76" spans="1:32" s="16" customFormat="1">
-      <c r="A76" s="39">
+      <c r="A76" s="38">
         <v>67</v>
       </c>
       <c r="B76" s="4" t="s">
@@ -2900,7 +2908,7 @@
       <c r="AF76" s="13"/>
     </row>
     <row r="77" spans="1:32" s="16" customFormat="1">
-      <c r="A77" s="39">
+      <c r="A77" s="38">
         <v>68</v>
       </c>
       <c r="B77" s="4" t="s">
@@ -2914,7 +2922,7 @@
       <c r="AF77" s="13"/>
     </row>
     <row r="78" spans="1:32" s="16" customFormat="1">
-      <c r="A78" s="39">
+      <c r="A78" s="38">
         <v>69</v>
       </c>
       <c r="B78" s="4" t="s">
@@ -2928,7 +2936,7 @@
       <c r="AF78" s="13"/>
     </row>
     <row r="79" spans="1:32" s="16" customFormat="1">
-      <c r="A79" s="39">
+      <c r="A79" s="38">
         <v>70</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -2942,7 +2950,7 @@
       <c r="AF79" s="13"/>
     </row>
     <row r="80" spans="1:32" s="16" customFormat="1">
-      <c r="A80" s="39">
+      <c r="A80" s="38">
         <v>71</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -2956,7 +2964,7 @@
       <c r="AF80" s="13"/>
     </row>
     <row r="81" spans="1:32" s="16" customFormat="1">
-      <c r="A81" s="39">
+      <c r="A81" s="38">
         <v>72</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -2970,7 +2978,7 @@
       <c r="AF81" s="13"/>
     </row>
     <row r="82" spans="1:32" s="16" customFormat="1">
-      <c r="A82" s="39">
+      <c r="A82" s="38">
         <v>73</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -2984,7 +2992,7 @@
       <c r="AF82" s="13"/>
     </row>
     <row r="83" spans="1:32" s="16" customFormat="1">
-      <c r="A83" s="39">
+      <c r="A83" s="38">
         <v>74</v>
       </c>
       <c r="B83" s="4" t="s">
@@ -2998,7 +3006,7 @@
       <c r="AF83" s="13"/>
     </row>
     <row r="84" spans="1:32" s="16" customFormat="1">
-      <c r="A84" s="39">
+      <c r="A84" s="38">
         <v>75</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -3012,7 +3020,7 @@
       <c r="AF84" s="13"/>
     </row>
     <row r="85" spans="1:32" s="16" customFormat="1">
-      <c r="A85" s="39">
+      <c r="A85" s="38">
         <v>76</v>
       </c>
       <c r="B85" s="4" t="s">
@@ -3026,7 +3034,7 @@
       <c r="AF85" s="13"/>
     </row>
     <row r="86" spans="1:32" s="16" customFormat="1">
-      <c r="A86" s="39">
+      <c r="A86" s="38">
         <v>77</v>
       </c>
       <c r="B86" s="4" t="s">
@@ -3040,7 +3048,7 @@
       <c r="AF86" s="13"/>
     </row>
     <row r="87" spans="1:32" s="16" customFormat="1">
-      <c r="A87" s="39">
+      <c r="A87" s="38">
         <v>78</v>
       </c>
       <c r="B87" s="4" t="s">
@@ -3054,7 +3062,7 @@
       <c r="AF87" s="13"/>
     </row>
     <row r="88" spans="1:32" s="16" customFormat="1">
-      <c r="A88" s="39">
+      <c r="A88" s="38">
         <v>79</v>
       </c>
       <c r="B88" s="4" t="s">
@@ -3068,7 +3076,7 @@
       <c r="AF88" s="13"/>
     </row>
     <row r="89" spans="1:32" s="16" customFormat="1">
-      <c r="A89" s="39">
+      <c r="A89" s="38">
         <v>80</v>
       </c>
       <c r="B89" s="4" t="s">
@@ -3082,7 +3090,7 @@
       <c r="AF89" s="13"/>
     </row>
     <row r="90" spans="1:32" s="16" customFormat="1">
-      <c r="A90" s="39">
+      <c r="A90" s="38">
         <v>81</v>
       </c>
       <c r="B90" s="4" t="s">
@@ -3096,7 +3104,7 @@
       <c r="AF90" s="13"/>
     </row>
     <row r="91" spans="1:32" s="16" customFormat="1">
-      <c r="A91" s="39">
+      <c r="A91" s="38">
         <v>82</v>
       </c>
       <c r="B91" s="4" t="s">
@@ -3110,7 +3118,7 @@
       <c r="AF91" s="13"/>
     </row>
     <row r="92" spans="1:32" s="16" customFormat="1">
-      <c r="A92" s="39">
+      <c r="A92" s="38">
         <v>83</v>
       </c>
       <c r="B92" s="4" t="s">
@@ -3124,7 +3132,7 @@
       <c r="AF92" s="13"/>
     </row>
     <row r="93" spans="1:32" s="16" customFormat="1">
-      <c r="A93" s="39">
+      <c r="A93" s="38">
         <v>84</v>
       </c>
       <c r="B93" s="4" t="s">
@@ -3138,7 +3146,7 @@
       <c r="AF93" s="13"/>
     </row>
     <row r="94" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A94" s="39"/>
+      <c r="A94" s="38"/>
       <c r="B94" s="2"/>
       <c r="C94" s="15"/>
       <c r="AD94" s="13"/>
@@ -3146,9 +3154,9 @@
       <c r="AF94" s="13"/>
     </row>
     <row r="95" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A95" s="39"/>
+      <c r="A95" s="38"/>
       <c r="B95" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C95" s="15"/>
       <c r="AD95" s="13"/>
@@ -3156,7 +3164,7 @@
       <c r="AF95" s="13"/>
     </row>
     <row r="96" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A96" s="39"/>
+      <c r="A96" s="38"/>
       <c r="B96" s="2"/>
       <c r="C96" s="15"/>
       <c r="AD96" s="13"/>
@@ -3164,9 +3172,9 @@
       <c r="AF96" s="13"/>
     </row>
     <row r="97" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A97" s="39"/>
+      <c r="A97" s="38"/>
       <c r="B97" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C97" s="15"/>
       <c r="AD97" s="13"/>
@@ -3174,11 +3182,11 @@
       <c r="AF97" s="13"/>
     </row>
     <row r="98" spans="1:32" s="16" customFormat="1">
-      <c r="A98" s="39">
+      <c r="A98" s="38">
         <v>1</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C98" s="15">
         <v>0.8</v>
@@ -3188,11 +3196,11 @@
       <c r="AF98" s="13"/>
     </row>
     <row r="99" spans="1:32" s="16" customFormat="1">
-      <c r="A99" s="39">
+      <c r="A99" s="38">
         <v>2</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C99" s="15">
         <v>0.8</v>
@@ -3202,11 +3210,11 @@
       <c r="AF99" s="13"/>
     </row>
     <row r="100" spans="1:32" s="16" customFormat="1">
-      <c r="A100" s="39">
+      <c r="A100" s="38">
         <v>3</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C100" s="15">
         <v>0.8</v>
@@ -3216,11 +3224,11 @@
       <c r="AF100" s="13"/>
     </row>
     <row r="101" spans="1:32" s="16" customFormat="1">
-      <c r="A101" s="39">
+      <c r="A101" s="38">
         <v>4</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C101" s="15">
         <v>0.9</v>
@@ -3230,11 +3238,11 @@
       <c r="AF101" s="13"/>
     </row>
     <row r="102" spans="1:32" s="16" customFormat="1">
-      <c r="A102" s="39">
+      <c r="A102" s="38">
         <v>5</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C102" s="15">
         <v>0.8</v>
@@ -3244,11 +3252,11 @@
       <c r="AF102" s="13"/>
     </row>
     <row r="103" spans="1:32" s="16" customFormat="1">
-      <c r="A103" s="39">
+      <c r="A103" s="38">
         <v>6</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C103" s="15">
         <v>0.9</v>
@@ -3258,11 +3266,11 @@
       <c r="AF103" s="13"/>
     </row>
     <row r="104" spans="1:32" s="16" customFormat="1">
-      <c r="A104" s="39">
+      <c r="A104" s="38">
         <v>7</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C104" s="15">
         <v>0.9</v>
@@ -3272,11 +3280,11 @@
       <c r="AF104" s="13"/>
     </row>
     <row r="105" spans="1:32" s="16" customFormat="1">
-      <c r="A105" s="39">
+      <c r="A105" s="38">
         <v>8</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C105" s="15">
         <v>1</v>
@@ -3286,11 +3294,11 @@
       <c r="AF105" s="13"/>
     </row>
     <row r="106" spans="1:32" s="16" customFormat="1">
-      <c r="A106" s="39">
+      <c r="A106" s="38">
         <v>9</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C106" s="15">
         <v>1.1000000000000001</v>
@@ -3300,11 +3308,11 @@
       <c r="AF106" s="13"/>
     </row>
     <row r="107" spans="1:32" s="16" customFormat="1">
-      <c r="A107" s="39">
+      <c r="A107" s="38">
         <v>10</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C107" s="15">
         <v>1.1000000000000001</v>
@@ -3314,11 +3322,11 @@
       <c r="AF107" s="13"/>
     </row>
     <row r="108" spans="1:32" s="16" customFormat="1">
-      <c r="A108" s="39">
+      <c r="A108" s="38">
         <v>11</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C108" s="15">
         <v>1.1000000000000001</v>
@@ -3328,11 +3336,11 @@
       <c r="AF108" s="13"/>
     </row>
     <row r="109" spans="1:32" s="16" customFormat="1">
-      <c r="A109" s="39">
+      <c r="A109" s="38">
         <v>12</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C109" s="15">
         <v>1</v>
@@ -3342,11 +3350,11 @@
       <c r="AF109" s="13"/>
     </row>
     <row r="110" spans="1:32" s="16" customFormat="1">
-      <c r="A110" s="39">
+      <c r="A110" s="38">
         <v>13</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C110" s="15">
         <v>1</v>
@@ -3356,11 +3364,11 @@
       <c r="AF110" s="13"/>
     </row>
     <row r="111" spans="1:32" s="16" customFormat="1">
-      <c r="A111" s="39">
+      <c r="A111" s="38">
         <v>14</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C111" s="15">
         <v>1</v>
@@ -3370,11 +3378,11 @@
       <c r="AF111" s="13"/>
     </row>
     <row r="112" spans="1:32" s="16" customFormat="1">
-      <c r="A112" s="39">
+      <c r="A112" s="38">
         <v>15</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C112" s="15">
         <v>1</v>
@@ -3384,11 +3392,11 @@
       <c r="AF112" s="13"/>
     </row>
     <row r="113" spans="1:32" s="16" customFormat="1">
-      <c r="A113" s="39">
+      <c r="A113" s="38">
         <v>16</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C113" s="15">
         <v>1</v>
@@ -3398,11 +3406,11 @@
       <c r="AF113" s="13"/>
     </row>
     <row r="114" spans="1:32" s="16" customFormat="1">
-      <c r="A114" s="39">
+      <c r="A114" s="38">
         <v>17</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C114" s="15">
         <v>1</v>
@@ -3412,11 +3420,11 @@
       <c r="AF114" s="13"/>
     </row>
     <row r="115" spans="1:32" s="16" customFormat="1">
-      <c r="A115" s="39">
+      <c r="A115" s="38">
         <v>18</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C115" s="15">
         <v>1</v>
@@ -3426,11 +3434,11 @@
       <c r="AF115" s="13"/>
     </row>
     <row r="116" spans="1:32" s="16" customFormat="1">
-      <c r="A116" s="39">
+      <c r="A116" s="38">
         <v>19</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C116" s="15">
         <v>1</v>
@@ -3440,11 +3448,11 @@
       <c r="AF116" s="13"/>
     </row>
     <row r="117" spans="1:32" s="16" customFormat="1">
-      <c r="A117" s="39">
+      <c r="A117" s="38">
         <v>20</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C117" s="15">
         <v>1.2</v>
@@ -3454,11 +3462,11 @@
       <c r="AF117" s="13"/>
     </row>
     <row r="118" spans="1:32" s="16" customFormat="1">
-      <c r="A118" s="39">
+      <c r="A118" s="38">
         <v>21</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C118" s="15">
         <v>0.8</v>
@@ -3468,7 +3476,7 @@
       <c r="AF118" s="13"/>
     </row>
     <row r="119" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A119" s="39"/>
+      <c r="A119" s="38"/>
       <c r="B119" s="6"/>
       <c r="C119" s="15"/>
       <c r="AD119" s="13"/>
@@ -3476,9 +3484,9 @@
       <c r="AF119" s="13"/>
     </row>
     <row r="120" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A120" s="39"/>
+      <c r="A120" s="38"/>
       <c r="B120" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C120" s="15"/>
       <c r="AD120" s="13"/>
@@ -3486,7 +3494,7 @@
       <c r="AF120" s="13"/>
     </row>
     <row r="121" spans="1:32" s="16" customFormat="1" ht="18">
-      <c r="A121" s="39"/>
+      <c r="A121" s="38"/>
       <c r="B121" s="4"/>
       <c r="C121" s="26">
         <v>500</v>
@@ -3511,7 +3519,7 @@
       <c r="AF121" s="13"/>
     </row>
     <row r="122" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A122" s="39"/>
+      <c r="A122" s="38"/>
       <c r="B122" s="2"/>
       <c r="C122" s="15"/>
       <c r="AD122" s="13"/>
@@ -3519,9 +3527,9 @@
       <c r="AF122" s="13"/>
     </row>
     <row r="123" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A123" s="39"/>
+      <c r="A123" s="38"/>
       <c r="B123" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C123" s="15"/>
       <c r="AD123" s="13"/>
@@ -3529,7 +3537,7 @@
       <c r="AF123" s="13"/>
     </row>
     <row r="124" spans="1:32" s="16" customFormat="1">
-      <c r="A124" s="39"/>
+      <c r="A124" s="38"/>
       <c r="B124" s="4"/>
       <c r="C124" s="15">
         <v>1</v>
@@ -3539,7 +3547,7 @@
       <c r="AF124" s="13"/>
     </row>
     <row r="125" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A125" s="39"/>
+      <c r="A125" s="38"/>
       <c r="B125" s="2"/>
       <c r="C125" s="15"/>
       <c r="AD125" s="13"/>
@@ -3547,9 +3555,9 @@
       <c r="AF125" s="13"/>
     </row>
     <row r="126" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A126" s="39"/>
+      <c r="A126" s="38"/>
       <c r="B126" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C126" s="15"/>
       <c r="AD126" s="13"/>
@@ -3557,7 +3565,7 @@
       <c r="AF126" s="13"/>
     </row>
     <row r="127" spans="1:32" s="16" customFormat="1">
-      <c r="A127" s="39">
+      <c r="A127" s="38">
         <v>1</v>
       </c>
       <c r="B127" s="3">
@@ -3571,7 +3579,7 @@
       <c r="AF127" s="13"/>
     </row>
     <row r="128" spans="1:32" s="16" customFormat="1">
-      <c r="A128" s="39">
+      <c r="A128" s="38">
         <v>2</v>
       </c>
       <c r="B128" s="3">
@@ -3585,7 +3593,7 @@
       <c r="AF128" s="13"/>
     </row>
     <row r="129" spans="1:32" s="16" customFormat="1">
-      <c r="A129" s="39">
+      <c r="A129" s="38">
         <v>3</v>
       </c>
       <c r="B129" s="3">
@@ -3599,7 +3607,7 @@
       <c r="AF129" s="13"/>
     </row>
     <row r="130" spans="1:32" s="16" customFormat="1">
-      <c r="A130" s="39">
+      <c r="A130" s="38">
         <v>4</v>
       </c>
       <c r="B130" s="3">
@@ -3613,7 +3621,7 @@
       <c r="AF130" s="13"/>
     </row>
     <row r="131" spans="1:32" s="16" customFormat="1">
-      <c r="A131" s="39">
+      <c r="A131" s="38">
         <v>5</v>
       </c>
       <c r="B131" s="3">
@@ -3627,7 +3635,7 @@
       <c r="AF131" s="13"/>
     </row>
     <row r="132" spans="1:32" s="16" customFormat="1">
-      <c r="A132" s="39">
+      <c r="A132" s="38">
         <v>6</v>
       </c>
       <c r="B132" s="3">
@@ -3641,7 +3649,7 @@
       <c r="AF132" s="13"/>
     </row>
     <row r="133" spans="1:32" s="16" customFormat="1">
-      <c r="A133" s="39">
+      <c r="A133" s="38">
         <v>7</v>
       </c>
       <c r="B133" s="3">
@@ -3655,7 +3663,7 @@
       <c r="AF133" s="13"/>
     </row>
     <row r="134" spans="1:32" s="16" customFormat="1">
-      <c r="A134" s="39">
+      <c r="A134" s="38">
         <v>8</v>
       </c>
       <c r="B134" s="3">
@@ -3669,7 +3677,7 @@
       <c r="AF134" s="13"/>
     </row>
     <row r="135" spans="1:32" s="16" customFormat="1">
-      <c r="A135" s="39">
+      <c r="A135" s="38">
         <v>9</v>
       </c>
       <c r="B135" s="3">
@@ -3683,7 +3691,7 @@
       <c r="AF135" s="13"/>
     </row>
     <row r="136" spans="1:32" s="16" customFormat="1">
-      <c r="A136" s="39">
+      <c r="A136" s="38">
         <v>10</v>
       </c>
       <c r="B136" s="3">
@@ -3697,7 +3705,7 @@
       <c r="AF136" s="13"/>
     </row>
     <row r="137" spans="1:32" s="16" customFormat="1">
-      <c r="A137" s="39">
+      <c r="A137" s="38">
         <v>11</v>
       </c>
       <c r="B137" s="3">
@@ -3711,7 +3719,7 @@
       <c r="AF137" s="13"/>
     </row>
     <row r="138" spans="1:32" s="16" customFormat="1">
-      <c r="A138" s="39">
+      <c r="A138" s="38">
         <v>12</v>
       </c>
       <c r="B138" s="3">
@@ -3725,7 +3733,7 @@
       <c r="AF138" s="13"/>
     </row>
     <row r="139" spans="1:32" s="16" customFormat="1">
-      <c r="A139" s="39">
+      <c r="A139" s="38">
         <v>13</v>
       </c>
       <c r="B139" s="3">
@@ -3739,7 +3747,7 @@
       <c r="AF139" s="13"/>
     </row>
     <row r="140" spans="1:32" s="16" customFormat="1">
-      <c r="A140" s="39">
+      <c r="A140" s="38">
         <v>14</v>
       </c>
       <c r="B140" s="3">
@@ -3753,7 +3761,7 @@
       <c r="AF140" s="13"/>
     </row>
     <row r="141" spans="1:32" s="16" customFormat="1">
-      <c r="A141" s="39">
+      <c r="A141" s="38">
         <v>15</v>
       </c>
       <c r="B141" s="3">
@@ -3767,7 +3775,7 @@
       <c r="AF141" s="13"/>
     </row>
     <row r="142" spans="1:32" s="16" customFormat="1">
-      <c r="A142" s="39">
+      <c r="A142" s="38">
         <v>16</v>
       </c>
       <c r="B142" s="3">
@@ -3781,7 +3789,7 @@
       <c r="AF142" s="13"/>
     </row>
     <row r="143" spans="1:32" s="16" customFormat="1">
-      <c r="A143" s="39">
+      <c r="A143" s="38">
         <v>17</v>
       </c>
       <c r="B143" s="3">
@@ -3795,7 +3803,7 @@
       <c r="AF143" s="13"/>
     </row>
     <row r="144" spans="1:32" s="16" customFormat="1">
-      <c r="A144" s="39">
+      <c r="A144" s="38">
         <v>18</v>
       </c>
       <c r="B144" s="3">
@@ -3809,7 +3817,7 @@
       <c r="AF144" s="13"/>
     </row>
     <row r="145" spans="1:32" s="16" customFormat="1">
-      <c r="A145" s="39">
+      <c r="A145" s="38">
         <v>19</v>
       </c>
       <c r="B145" s="3">
@@ -3823,7 +3831,7 @@
       <c r="AF145" s="13"/>
     </row>
     <row r="146" spans="1:32" s="16" customFormat="1">
-      <c r="A146" s="39">
+      <c r="A146" s="38">
         <v>20</v>
       </c>
       <c r="B146" s="3">
@@ -3837,7 +3845,7 @@
       <c r="AF146" s="13"/>
     </row>
     <row r="147" spans="1:32" s="16" customFormat="1">
-      <c r="A147" s="39">
+      <c r="A147" s="38">
         <v>21</v>
       </c>
       <c r="B147" s="3">
@@ -3851,7 +3859,7 @@
       <c r="AF147" s="13"/>
     </row>
     <row r="148" spans="1:32" s="16" customFormat="1">
-      <c r="A148" s="39">
+      <c r="A148" s="38">
         <v>22</v>
       </c>
       <c r="B148" s="3">
@@ -3865,7 +3873,7 @@
       <c r="AF148" s="13"/>
     </row>
     <row r="149" spans="1:32" s="16" customFormat="1">
-      <c r="A149" s="39">
+      <c r="A149" s="38">
         <v>23</v>
       </c>
       <c r="B149" s="3">
@@ -3879,7 +3887,7 @@
       <c r="AF149" s="13"/>
     </row>
     <row r="150" spans="1:32" s="16" customFormat="1">
-      <c r="A150" s="39">
+      <c r="A150" s="38">
         <v>24</v>
       </c>
       <c r="B150" s="3">
@@ -3893,7 +3901,7 @@
       <c r="AF150" s="13"/>
     </row>
     <row r="151" spans="1:32" s="16" customFormat="1">
-      <c r="A151" s="39">
+      <c r="A151" s="38">
         <v>25</v>
       </c>
       <c r="B151" s="3">
@@ -3907,7 +3915,7 @@
       <c r="AF151" s="13"/>
     </row>
     <row r="152" spans="1:32" s="16" customFormat="1">
-      <c r="A152" s="39">
+      <c r="A152" s="38">
         <v>26</v>
       </c>
       <c r="B152" s="3">
@@ -3921,7 +3929,7 @@
       <c r="AF152" s="13"/>
     </row>
     <row r="153" spans="1:32" s="16" customFormat="1">
-      <c r="A153" s="39">
+      <c r="A153" s="38">
         <v>27</v>
       </c>
       <c r="B153" s="3">
@@ -3935,7 +3943,7 @@
       <c r="AF153" s="13"/>
     </row>
     <row r="154" spans="1:32" s="16" customFormat="1">
-      <c r="A154" s="39">
+      <c r="A154" s="38">
         <v>28</v>
       </c>
       <c r="B154" s="3">
@@ -3949,7 +3957,7 @@
       <c r="AF154" s="13"/>
     </row>
     <row r="155" spans="1:32" s="16" customFormat="1">
-      <c r="A155" s="39">
+      <c r="A155" s="38">
         <v>29</v>
       </c>
       <c r="B155" s="3">
@@ -3963,7 +3971,7 @@
       <c r="AF155" s="13"/>
     </row>
     <row r="156" spans="1:32" s="16" customFormat="1">
-      <c r="A156" s="39">
+      <c r="A156" s="38">
         <v>30</v>
       </c>
       <c r="B156" s="3">
@@ -3977,7 +3985,7 @@
       <c r="AF156" s="13"/>
     </row>
     <row r="157" spans="1:32" s="16" customFormat="1">
-      <c r="A157" s="39">
+      <c r="A157" s="38">
         <v>31</v>
       </c>
       <c r="B157" s="3" t="s">
@@ -3991,7 +3999,7 @@
       <c r="AF157" s="13"/>
     </row>
     <row r="158" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A158" s="39"/>
+      <c r="A158" s="38"/>
       <c r="B158" s="7"/>
       <c r="C158" s="15"/>
       <c r="AD158" s="13"/>
@@ -3999,9 +4007,9 @@
       <c r="AF158" s="13"/>
     </row>
     <row r="159" spans="1:32" s="16" customFormat="1" ht="30">
-      <c r="A159" s="39"/>
+      <c r="A159" s="38"/>
       <c r="B159" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C159" s="15"/>
       <c r="AD159" s="13"/>
@@ -4009,7 +4017,7 @@
       <c r="AF159" s="13"/>
     </row>
     <row r="160" spans="1:32" s="16" customFormat="1">
-      <c r="A160" s="39">
+      <c r="A160" s="38">
         <v>1</v>
       </c>
       <c r="B160" s="4" t="s">
@@ -4023,7 +4031,7 @@
       <c r="AF160" s="13"/>
     </row>
     <row r="161" spans="1:32" s="16" customFormat="1">
-      <c r="A161" s="39">
+      <c r="A161" s="38">
         <v>2</v>
       </c>
       <c r="B161" s="4" t="s">
@@ -4037,7 +4045,7 @@
       <c r="AF161" s="13"/>
     </row>
     <row r="162" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A162" s="39"/>
+      <c r="A162" s="38"/>
       <c r="B162" s="2"/>
       <c r="C162" s="15"/>
       <c r="AD162" s="13"/>
@@ -4045,9 +4053,9 @@
       <c r="AF162" s="13"/>
     </row>
     <row r="163" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A163" s="39"/>
+      <c r="A163" s="38"/>
       <c r="B163" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C163" s="15"/>
       <c r="AD163" s="13"/>
@@ -4055,7 +4063,7 @@
       <c r="AF163" s="13"/>
     </row>
     <row r="164" spans="1:32" s="16" customFormat="1">
-      <c r="A164" s="39">
+      <c r="A164" s="38">
         <v>1</v>
       </c>
       <c r="B164" s="5">
@@ -4069,7 +4077,7 @@
       <c r="AF164" s="13"/>
     </row>
     <row r="165" spans="1:32" s="16" customFormat="1">
-      <c r="A165" s="39">
+      <c r="A165" s="38">
         <v>2</v>
       </c>
       <c r="B165" s="5">
@@ -4083,7 +4091,7 @@
       <c r="AF165" s="13"/>
     </row>
     <row r="166" spans="1:32" s="16" customFormat="1">
-      <c r="A166" s="39">
+      <c r="A166" s="38">
         <v>3</v>
       </c>
       <c r="B166" s="5">
@@ -4097,7 +4105,7 @@
       <c r="AF166" s="13"/>
     </row>
     <row r="167" spans="1:32" s="16" customFormat="1">
-      <c r="A167" s="39">
+      <c r="A167" s="38">
         <v>4</v>
       </c>
       <c r="B167" s="5" t="s">
@@ -4111,7 +4119,7 @@
       <c r="AF167" s="13"/>
     </row>
     <row r="168" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A168" s="39"/>
+      <c r="A168" s="38"/>
       <c r="B168" s="10"/>
       <c r="C168" s="15"/>
       <c r="AD168" s="13"/>
@@ -4119,9 +4127,9 @@
       <c r="AF168" s="13"/>
     </row>
     <row r="169" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A169" s="39"/>
+      <c r="A169" s="38"/>
       <c r="B169" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C169" s="15"/>
       <c r="AD169" s="13"/>
@@ -4129,11 +4137,11 @@
       <c r="AF169" s="13"/>
     </row>
     <row r="170" spans="1:32" s="16" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A170" s="39">
+      <c r="A170" s="38">
         <v>1</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C170" s="15">
         <v>1</v>
@@ -4143,11 +4151,11 @@
       <c r="AF170" s="13"/>
     </row>
     <row r="171" spans="1:32" s="16" customFormat="1" ht="43.5" customHeight="1">
-      <c r="A171" s="39">
+      <c r="A171" s="38">
         <v>2</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C171" s="15">
         <v>1</v>
@@ -4157,11 +4165,11 @@
       <c r="AF171" s="13"/>
     </row>
     <row r="172" spans="1:32" s="16" customFormat="1" ht="46.5" customHeight="1">
-      <c r="A172" s="39">
+      <c r="A172" s="38">
         <v>3</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C172" s="15">
         <v>1</v>
@@ -4171,11 +4179,11 @@
       <c r="AF172" s="13"/>
     </row>
     <row r="173" spans="1:32" s="16" customFormat="1" ht="45" customHeight="1">
-      <c r="A173" s="39">
+      <c r="A173" s="38">
         <v>4</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C173" s="15">
         <v>0.9</v>
@@ -4185,11 +4193,11 @@
       <c r="AF173" s="13"/>
     </row>
     <row r="174" spans="1:32" s="16" customFormat="1" ht="45" customHeight="1">
-      <c r="A174" s="39">
+      <c r="A174" s="38">
         <v>5</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C174" s="15">
         <v>1</v>
@@ -4199,11 +4207,11 @@
       <c r="AF174" s="13"/>
     </row>
     <row r="175" spans="1:32" s="16" customFormat="1" ht="60" customHeight="1">
-      <c r="A175" s="39">
+      <c r="A175" s="38">
         <v>6</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C175" s="15">
         <v>1</v>
@@ -4213,11 +4221,11 @@
       <c r="AF175" s="13"/>
     </row>
     <row r="176" spans="1:32" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A176" s="39">
+      <c r="A176" s="38">
         <v>7</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C176" s="15">
         <v>0.8</v>
@@ -4227,11 +4235,11 @@
       <c r="AF176" s="13"/>
     </row>
     <row r="177" spans="1:32" s="16" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A177" s="39">
+      <c r="A177" s="38">
         <v>8</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C177" s="15">
         <v>1</v>
@@ -4241,11 +4249,11 @@
       <c r="AF177" s="13"/>
     </row>
     <row r="178" spans="1:32" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A178" s="39">
+      <c r="A178" s="38">
         <v>9</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C178" s="15">
         <v>1</v>
@@ -4255,11 +4263,11 @@
       <c r="AF178" s="13"/>
     </row>
     <row r="179" spans="1:32" s="16" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A179" s="39">
+      <c r="A179" s="38">
         <v>10</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C179" s="15">
         <v>1</v>
@@ -4269,11 +4277,11 @@
       <c r="AF179" s="13"/>
     </row>
     <row r="180" spans="1:32" s="16" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A180" s="39">
+      <c r="A180" s="38">
         <v>11</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C180" s="15">
         <v>1</v>
@@ -4283,11 +4291,11 @@
       <c r="AF180" s="13"/>
     </row>
     <row r="181" spans="1:32" s="16" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A181" s="39">
+      <c r="A181" s="38">
         <v>12</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C181" s="15">
         <v>0.9</v>
@@ -4297,11 +4305,11 @@
       <c r="AF181" s="13"/>
     </row>
     <row r="182" spans="1:32" s="16" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A182" s="39">
+      <c r="A182" s="38">
         <v>13</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C182" s="15">
         <v>0.8</v>
@@ -4311,11 +4319,11 @@
       <c r="AF182" s="13"/>
     </row>
     <row r="183" spans="1:32" s="16" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A183" s="39">
+      <c r="A183" s="38">
         <v>14</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C183" s="15">
         <v>0.8</v>
@@ -4325,11 +4333,11 @@
       <c r="AF183" s="13"/>
     </row>
     <row r="184" spans="1:32" s="16" customFormat="1" ht="63" customHeight="1">
-      <c r="A184" s="39">
+      <c r="A184" s="38">
         <v>15</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C184" s="15">
         <v>1</v>
@@ -4339,11 +4347,11 @@
       <c r="AF184" s="13"/>
     </row>
     <row r="185" spans="1:32" s="16" customFormat="1">
-      <c r="A185" s="39">
+      <c r="A185" s="38">
         <v>16</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C185" s="15">
         <v>0.9</v>
@@ -4353,7 +4361,7 @@
       <c r="AF185" s="13"/>
     </row>
     <row r="186" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A186" s="39"/>
+      <c r="A186" s="38"/>
       <c r="B186" s="2"/>
       <c r="C186" s="15"/>
       <c r="AD186" s="13"/>
@@ -4361,9 +4369,9 @@
       <c r="AF186" s="13"/>
     </row>
     <row r="187" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A187" s="39"/>
+      <c r="A187" s="38"/>
       <c r="B187" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C187" s="15"/>
       <c r="AD187" s="13"/>
@@ -4371,7 +4379,7 @@
       <c r="AF187" s="13"/>
     </row>
     <row r="188" spans="1:32" s="16" customFormat="1">
-      <c r="A188" s="39"/>
+      <c r="A188" s="38"/>
       <c r="B188" s="4" t="s">
         <v>112</v>
       </c>
@@ -4381,11 +4389,11 @@
       <c r="AF188" s="13"/>
     </row>
     <row r="189" spans="1:32" s="16" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A189" s="39">
+      <c r="A189" s="38">
         <v>1</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C189" s="15">
         <v>1.8</v>
@@ -4395,11 +4403,11 @@
       <c r="AF189" s="13"/>
     </row>
     <row r="190" spans="1:32" s="16" customFormat="1" ht="28">
-      <c r="A190" s="39">
+      <c r="A190" s="38">
         <v>2</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C190" s="15">
         <v>1</v>
@@ -4409,11 +4417,11 @@
       <c r="AF190" s="13"/>
     </row>
     <row r="191" spans="1:32" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A191" s="39">
+      <c r="A191" s="38">
         <v>3</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C191" s="15">
         <v>0.7</v>
@@ -4423,7 +4431,7 @@
       <c r="AF191" s="13"/>
     </row>
     <row r="192" spans="1:32" s="16" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A192" s="39"/>
+      <c r="A192" s="38"/>
       <c r="B192" s="4" t="s">
         <v>113</v>
       </c>
@@ -4459,11 +4467,11 @@
       <c r="AF192" s="13"/>
     </row>
     <row r="193" spans="1:32" s="16" customFormat="1">
-      <c r="A193" s="39">
+      <c r="A193" s="38">
         <v>1</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C193" s="18">
         <v>0.6</v>
@@ -4502,11 +4510,11 @@
       <c r="AF193" s="13"/>
     </row>
     <row r="194" spans="1:32" s="16" customFormat="1" ht="46.5" customHeight="1">
-      <c r="A194" s="39">
+      <c r="A194" s="38">
         <v>2</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C194" s="18">
         <v>0.75</v>
@@ -4545,11 +4553,11 @@
       <c r="AF194" s="13"/>
     </row>
     <row r="195" spans="1:32" s="16" customFormat="1" ht="46.5" customHeight="1">
-      <c r="A195" s="39">
+      <c r="A195" s="38">
         <v>3</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C195" s="18">
         <v>0.4</v>
@@ -4588,11 +4596,11 @@
       <c r="AF195" s="13"/>
     </row>
     <row r="196" spans="1:32" s="16" customFormat="1">
-      <c r="A196" s="39">
+      <c r="A196" s="38">
         <v>4</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C196" s="18">
         <v>0.8</v>
@@ -4631,11 +4639,11 @@
       <c r="AF196" s="13"/>
     </row>
     <row r="197" spans="1:32" s="16" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A197" s="39">
+      <c r="A197" s="38">
         <v>5</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C197" s="18">
         <v>0.28000000000000003</v>
@@ -4674,11 +4682,11 @@
       <c r="AF197" s="13"/>
     </row>
     <row r="198" spans="1:32" s="16" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A198" s="39">
+      <c r="A198" s="38">
         <v>6</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C198" s="18">
         <v>0.53</v>
@@ -4717,11 +4725,11 @@
       <c r="AF198" s="13"/>
     </row>
     <row r="199" spans="1:32" s="16" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A199" s="39">
+      <c r="A199" s="38">
         <v>7</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C199" s="18">
         <v>0.41</v>
@@ -4760,11 +4768,11 @@
       <c r="AF199" s="13"/>
     </row>
     <row r="200" spans="1:32" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A200" s="39">
+      <c r="A200" s="38">
         <v>8</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C200" s="18">
         <v>0.31</v>
@@ -4803,11 +4811,11 @@
       <c r="AF200" s="13"/>
     </row>
     <row r="201" spans="1:32" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A201" s="39">
+      <c r="A201" s="38">
         <v>9</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C201" s="18">
         <v>0.43</v>
@@ -4846,11 +4854,11 @@
       <c r="AF201" s="13"/>
     </row>
     <row r="202" spans="1:32" s="16" customFormat="1" ht="18" customHeight="1">
-      <c r="A202" s="39">
+      <c r="A202" s="38">
         <v>10</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C202" s="18">
         <v>0.73</v>
@@ -4889,11 +4897,11 @@
       <c r="AF202" s="13"/>
     </row>
     <row r="203" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A203" s="39">
+      <c r="A203" s="38">
         <v>11</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C203" s="18">
         <v>0.35</v>
@@ -4932,11 +4940,11 @@
       <c r="AF203" s="13"/>
     </row>
     <row r="204" spans="1:32" s="16" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A204" s="39">
+      <c r="A204" s="38">
         <v>12</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C204" s="18">
         <v>0.31</v>
@@ -4975,11 +4983,11 @@
       <c r="AF204" s="13"/>
     </row>
     <row r="205" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A205" s="39">
+      <c r="A205" s="38">
         <v>13</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C205" s="18">
         <v>0.35</v>
@@ -5018,11 +5026,11 @@
       <c r="AF205" s="13"/>
     </row>
     <row r="206" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A206" s="39">
+      <c r="A206" s="38">
         <v>14</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C206" s="18">
         <v>0.32</v>
@@ -5061,11 +5069,11 @@
       <c r="AF206" s="13"/>
     </row>
     <row r="207" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A207" s="39">
+      <c r="A207" s="38">
         <v>15</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C207" s="18">
         <v>0.35</v>
@@ -5104,7 +5112,7 @@
       <c r="AF207" s="13"/>
     </row>
     <row r="208" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A208" s="39"/>
+      <c r="A208" s="38"/>
       <c r="B208" s="4"/>
       <c r="C208" s="18"/>
       <c r="D208" s="23"/>
@@ -5125,18 +5133,18 @@
       <c r="AE208" s="13"/>
       <c r="AF208" s="13"/>
     </row>
-    <row r="209" spans="1:32" s="42" customFormat="1" ht="14" customHeight="1">
-      <c r="A209" s="40"/>
-      <c r="B209" s="41" t="s">
-        <v>162</v>
+    <row r="209" spans="1:32" s="41" customFormat="1" ht="14" customHeight="1">
+      <c r="A209" s="39"/>
+      <c r="B209" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="C209" s="25"/>
-      <c r="AD209" s="43"/>
-      <c r="AE209" s="43"/>
-      <c r="AF209" s="43"/>
+      <c r="AD209" s="42"/>
+      <c r="AE209" s="42"/>
+      <c r="AF209" s="42"/>
     </row>
     <row r="210" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A210" s="39"/>
+      <c r="A210" s="38"/>
       <c r="B210" s="34"/>
       <c r="C210" s="15"/>
       <c r="AD210" s="13"/>
@@ -5144,9 +5152,9 @@
       <c r="AF210" s="13"/>
     </row>
     <row r="211" spans="1:32" s="16" customFormat="1" ht="15">
-      <c r="A211" s="39"/>
+      <c r="A211" s="38"/>
       <c r="B211" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C211" s="15"/>
       <c r="AD211" s="13"/>
@@ -5154,11 +5162,11 @@
       <c r="AF211" s="13"/>
     </row>
     <row r="212" spans="1:32" s="16" customFormat="1">
-      <c r="A212" s="39">
+      <c r="A212" s="38">
         <v>1</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C212" s="15">
         <v>0.8</v>
@@ -5168,11 +5176,11 @@
       <c r="AF212" s="13"/>
     </row>
     <row r="213" spans="1:32" s="16" customFormat="1" ht="28">
-      <c r="A213" s="39">
+      <c r="A213" s="38">
         <v>2</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C213" s="15">
         <v>1</v>
@@ -5182,11 +5190,11 @@
       <c r="AF213" s="13"/>
     </row>
     <row r="214" spans="1:32" s="16" customFormat="1" ht="28">
-      <c r="A214" s="39">
+      <c r="A214" s="38">
         <v>3</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C214" s="15">
         <v>1.2</v>
@@ -5196,11 +5204,11 @@
       <c r="AF214" s="13"/>
     </row>
     <row r="215" spans="1:32" s="16" customFormat="1" ht="28">
-      <c r="A215" s="39">
+      <c r="A215" s="38">
         <v>4</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C215" s="15">
         <v>1.5</v>
@@ -5210,11 +5218,11 @@
       <c r="AF215" s="13"/>
     </row>
     <row r="216" spans="1:32" s="16" customFormat="1" ht="28">
-      <c r="A216" s="39">
+      <c r="A216" s="38">
         <v>5</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C216" s="15">
         <v>2</v>
@@ -5224,11 +5232,11 @@
       <c r="AF216" s="13"/>
     </row>
     <row r="217" spans="1:32" s="16" customFormat="1" ht="28">
-      <c r="A217" s="39">
+      <c r="A217" s="38">
         <v>6</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C217" s="15">
         <v>2.2000000000000002</v>
@@ -5238,11 +5246,11 @@
       <c r="AF217" s="13"/>
     </row>
     <row r="218" spans="1:32" s="16" customFormat="1" ht="28">
-      <c r="A218" s="39">
+      <c r="A218" s="38">
         <v>7</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C218" s="15">
         <v>2.5</v>
@@ -5252,11 +5260,11 @@
       <c r="AF218" s="13"/>
     </row>
     <row r="219" spans="1:32" s="16" customFormat="1">
-      <c r="A219" s="39">
+      <c r="A219" s="38">
         <v>8</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C219" s="15">
         <v>3</v>
@@ -5266,7 +5274,7 @@
       <c r="AF219" s="13"/>
     </row>
     <row r="220" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A220" s="39"/>
+      <c r="A220" s="38"/>
       <c r="B220" s="2"/>
       <c r="C220" s="15"/>
       <c r="AD220" s="13"/>
@@ -5274,9 +5282,9 @@
       <c r="AF220" s="13"/>
     </row>
     <row r="221" spans="1:32" s="16" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A221" s="39"/>
+      <c r="A221" s="38"/>
       <c r="B221" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C221" s="15"/>
       <c r="AD221" s="13"/>
@@ -5284,7 +5292,7 @@
       <c r="AF221" s="13"/>
     </row>
     <row r="222" spans="1:32" s="16" customFormat="1">
-      <c r="A222" s="39">
+      <c r="A222" s="38">
         <v>1</v>
       </c>
       <c r="B222" s="11" t="s">
@@ -5296,7 +5304,7 @@
       <c r="AF222" s="13"/>
     </row>
     <row r="223" spans="1:32" s="16" customFormat="1">
-      <c r="A223" s="39"/>
+      <c r="A223" s="38"/>
       <c r="B223" s="11" t="s">
         <v>106</v>
       </c>
@@ -5308,7 +5316,7 @@
       <c r="AF223" s="13"/>
     </row>
     <row r="224" spans="1:32" s="16" customFormat="1">
-      <c r="A224" s="39">
+      <c r="A224" s="38">
         <v>2</v>
       </c>
       <c r="B224" s="11" t="s">
@@ -5320,7 +5328,7 @@
       <c r="AF224" s="13"/>
     </row>
     <row r="225" spans="1:32" s="16" customFormat="1">
-      <c r="A225" s="39"/>
+      <c r="A225" s="38"/>
       <c r="B225" s="11" t="s">
         <v>106</v>
       </c>
@@ -5332,7 +5340,7 @@
       <c r="AF225" s="13"/>
     </row>
     <row r="226" spans="1:32" s="16" customFormat="1">
-      <c r="A226" s="39">
+      <c r="A226" s="38">
         <v>3</v>
       </c>
       <c r="B226" s="11" t="s">
@@ -5344,7 +5352,7 @@
       <c r="AF226" s="13"/>
     </row>
     <row r="227" spans="1:32" s="16" customFormat="1">
-      <c r="A227" s="39"/>
+      <c r="A227" s="38"/>
       <c r="B227" s="11" t="s">
         <v>106</v>
       </c>
@@ -5356,7 +5364,7 @@
       <c r="AF227" s="13"/>
     </row>
     <row r="228" spans="1:32" s="16" customFormat="1">
-      <c r="A228" s="39">
+      <c r="A228" s="38">
         <v>4</v>
       </c>
       <c r="B228" s="11" t="s">
@@ -5368,7 +5376,7 @@
       <c r="AF228" s="13"/>
     </row>
     <row r="229" spans="1:32" s="16" customFormat="1">
-      <c r="A229" s="39"/>
+      <c r="A229" s="38"/>
       <c r="B229" s="11" t="s">
         <v>106</v>
       </c>
@@ -5380,7 +5388,7 @@
       <c r="AF229" s="13"/>
     </row>
     <row r="230" spans="1:32" s="16" customFormat="1">
-      <c r="A230" s="39">
+      <c r="A230" s="38">
         <v>5</v>
       </c>
       <c r="B230" s="11" t="s">
@@ -5392,7 +5400,7 @@
       <c r="AF230" s="13"/>
     </row>
     <row r="231" spans="1:32" s="16" customFormat="1">
-      <c r="A231" s="39"/>
+      <c r="A231" s="38"/>
       <c r="B231" s="11" t="s">
         <v>106</v>
       </c>
@@ -5404,7 +5412,7 @@
       <c r="AF231" s="13"/>
     </row>
     <row r="232" spans="1:32" s="16" customFormat="1">
-      <c r="A232" s="39">
+      <c r="A232" s="38">
         <v>6</v>
       </c>
       <c r="B232" s="11" t="s">
@@ -5416,7 +5424,7 @@
       <c r="AF232" s="13"/>
     </row>
     <row r="233" spans="1:32" s="16" customFormat="1">
-      <c r="A233" s="39"/>
+      <c r="A233" s="38"/>
       <c r="B233" s="11" t="s">
         <v>106</v>
       </c>
@@ -5428,7 +5436,7 @@
       <c r="AF233" s="13"/>
     </row>
     <row r="234" spans="1:32" s="16" customFormat="1" ht="15" thickBot="1">
-      <c r="A234" s="39"/>
+      <c r="A234" s="38"/>
       <c r="B234" s="12"/>
       <c r="C234" s="18"/>
       <c r="AD234" s="13"/>
@@ -5436,7 +5444,7 @@
       <c r="AF234" s="13"/>
     </row>
     <row r="236" spans="1:32" s="16" customFormat="1" ht="18">
-      <c r="A236" s="39"/>
+      <c r="A236" s="38"/>
       <c r="B236" s="14" t="s">
         <v>104</v>
       </c>
@@ -5456,7 +5464,7 @@
       <c r="AF236" s="13"/>
     </row>
     <row r="237" spans="1:32" s="16" customFormat="1">
-      <c r="A237" s="39"/>
+      <c r="A237" s="38"/>
       <c r="B237"/>
       <c r="D237" s="20"/>
       <c r="E237" s="20"/>
@@ -5467,7 +5475,7 @@
       <c r="AF237" s="13"/>
     </row>
     <row r="238" spans="1:32" s="16" customFormat="1" ht="18">
-      <c r="A238" s="39"/>
+      <c r="A238" s="38"/>
       <c r="B238" s="14" t="s">
         <v>105</v>
       </c>
@@ -5485,7 +5493,7 @@
       </c>
     </row>
     <row r="242" spans="1:32" s="16" customFormat="1" ht="18">
-      <c r="A242" s="39"/>
+      <c r="A242" s="38"/>
       <c r="B242" s="21" t="s">
         <v>114</v>
       </c>
@@ -5497,7 +5505,7 @@
       <c r="AF242" s="13"/>
     </row>
     <row r="243" spans="1:32" s="16" customFormat="1" ht="18">
-      <c r="A243" s="39"/>
+      <c r="A243" s="38"/>
       <c r="B243" s="21" t="s">
         <v>111</v>
       </c>
@@ -5542,7 +5550,7 @@
         <v>124</v>
       </c>
       <c r="C249" s="21" t="s">
-        <v>126</v>
+        <v>239</v>
       </c>
     </row>
     <row r="250" spans="1:32" ht="15">
@@ -5550,7 +5558,7 @@
         <v>125</v>
       </c>
       <c r="C250" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -5567,7 +5575,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5580,8 +5587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL386"/>
   <sheetViews>
-    <sheetView topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="B272" sqref="B272"/>
+    <sheetView topLeftCell="A323" workbookViewId="0">
+      <selection activeCell="D363" sqref="D363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5611,7 +5618,7 @@
     </row>
     <row r="4" spans="1:3" ht="15">
       <c r="B4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="15"/>
     </row>
@@ -5621,7 +5628,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -6731,7 +6738,7 @@
     </row>
     <row r="108" spans="1:3" ht="15">
       <c r="B108" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C108" s="15"/>
     </row>
@@ -7665,7 +7672,7 @@
     </row>
     <row r="194" spans="1:3" ht="15">
       <c r="B194" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C194" s="15"/>
     </row>
@@ -7675,7 +7682,7 @@
     </row>
     <row r="196" spans="1:3" ht="15">
       <c r="B196" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C196" s="15"/>
     </row>
@@ -7684,7 +7691,7 @@
         <v>1</v>
       </c>
       <c r="B197" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C197" s="25">
         <v>1.1000000000000001</v>
@@ -7695,7 +7702,7 @@
         <v>2</v>
       </c>
       <c r="B198" s="36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C198" s="25">
         <v>1.1000000000000001</v>
@@ -7706,7 +7713,7 @@
         <v>3</v>
       </c>
       <c r="B199" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C199" s="25">
         <v>1.1000000000000001</v>
@@ -7717,7 +7724,7 @@
         <v>4</v>
       </c>
       <c r="B200" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C200" s="25">
         <v>1.1000000000000001</v>
@@ -7728,7 +7735,7 @@
         <v>5</v>
       </c>
       <c r="B201" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C201" s="25">
         <v>1.1000000000000001</v>
@@ -7739,7 +7746,7 @@
         <v>6</v>
       </c>
       <c r="B202" s="36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C202" s="25">
         <v>1.1000000000000001</v>
@@ -7750,7 +7757,7 @@
         <v>7</v>
       </c>
       <c r="B203" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C203" s="25">
         <v>1.1000000000000001</v>
@@ -7761,7 +7768,7 @@
         <v>8</v>
       </c>
       <c r="B204" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C204" s="25">
         <v>1.1000000000000001</v>
@@ -7772,7 +7779,7 @@
         <v>9</v>
       </c>
       <c r="B205" s="36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C205" s="25">
         <v>1.1000000000000001</v>
@@ -7783,7 +7790,7 @@
         <v>10</v>
       </c>
       <c r="B206" s="36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C206" s="25">
         <v>1.1000000000000001</v>
@@ -7794,7 +7801,7 @@
         <v>11</v>
       </c>
       <c r="B207" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C207" s="25">
         <v>1.1000000000000001</v>
@@ -7805,7 +7812,7 @@
         <v>12</v>
       </c>
       <c r="B208" s="36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C208" s="25">
         <v>1.1000000000000001</v>
@@ -7816,7 +7823,7 @@
         <v>13</v>
       </c>
       <c r="B209" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C209" s="25">
         <v>1.1000000000000001</v>
@@ -7827,7 +7834,7 @@
         <v>14</v>
       </c>
       <c r="B210" s="36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C210" s="25">
         <v>1.1000000000000001</v>
@@ -7838,7 +7845,7 @@
         <v>15</v>
       </c>
       <c r="B211" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C211" s="25">
         <v>1.1000000000000001</v>
@@ -7849,7 +7856,7 @@
         <v>16</v>
       </c>
       <c r="B212" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C212" s="25">
         <v>1.1000000000000001</v>
@@ -7860,7 +7867,7 @@
         <v>17</v>
       </c>
       <c r="B213" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C213" s="25">
         <v>1.1000000000000001</v>
@@ -7871,7 +7878,7 @@
         <v>18</v>
       </c>
       <c r="B214" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C214" s="25">
         <v>1.1000000000000001</v>
@@ -7882,7 +7889,7 @@
         <v>19</v>
       </c>
       <c r="B215" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C215" s="25">
         <v>1.1000000000000001</v>
@@ -7893,7 +7900,7 @@
         <v>20</v>
       </c>
       <c r="B216" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C216" s="25">
         <v>1.1000000000000001</v>
@@ -7904,7 +7911,7 @@
         <v>21</v>
       </c>
       <c r="B217" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C217" s="25">
         <v>1.1000000000000001</v>
@@ -7915,7 +7922,7 @@
         <v>22</v>
       </c>
       <c r="B218" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C218" s="25">
         <v>1.1000000000000001</v>
@@ -7926,7 +7933,7 @@
         <v>23</v>
       </c>
       <c r="B219" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C219" s="25">
         <v>1.1000000000000001</v>
@@ -7937,7 +7944,7 @@
         <v>24</v>
       </c>
       <c r="B220" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C220" s="25">
         <v>1.1000000000000001</v>
@@ -7948,7 +7955,7 @@
         <v>25</v>
       </c>
       <c r="B221" s="36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C221" s="25">
         <v>1.1000000000000001</v>
@@ -7960,7 +7967,7 @@
     </row>
     <row r="223" spans="1:8" ht="15">
       <c r="B223" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C223" s="15"/>
     </row>
@@ -7981,7 +7988,7 @@
     </row>
     <row r="226" spans="1:3" ht="15">
       <c r="B226" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C226" s="15"/>
     </row>
@@ -7995,7 +8002,7 @@
     </row>
     <row r="229" spans="1:3" ht="15">
       <c r="B229" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C229" s="15"/>
     </row>
@@ -8006,7 +8013,7 @@
       <c r="B230" s="30">
         <v>1</v>
       </c>
-      <c r="C230" s="38">
+      <c r="C230" s="43">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -8017,7 +8024,7 @@
       <c r="B231" s="30">
         <v>2</v>
       </c>
-      <c r="C231" s="38"/>
+      <c r="C231" s="43"/>
     </row>
     <row r="232" spans="1:3">
       <c r="A232">
@@ -8026,7 +8033,7 @@
       <c r="B232" s="30">
         <v>3</v>
       </c>
-      <c r="C232" s="38"/>
+      <c r="C232" s="43"/>
     </row>
     <row r="233" spans="1:3">
       <c r="A233">
@@ -8035,7 +8042,7 @@
       <c r="B233" s="30">
         <v>4</v>
       </c>
-      <c r="C233" s="38"/>
+      <c r="C233" s="43"/>
     </row>
     <row r="234" spans="1:3">
       <c r="A234">
@@ -8044,7 +8051,7 @@
       <c r="B234" s="30">
         <v>5</v>
       </c>
-      <c r="C234" s="38"/>
+      <c r="C234" s="43"/>
     </row>
     <row r="235" spans="1:3">
       <c r="A235">
@@ -8053,7 +8060,7 @@
       <c r="B235" s="30">
         <v>6</v>
       </c>
-      <c r="C235" s="38"/>
+      <c r="C235" s="43"/>
     </row>
     <row r="236" spans="1:3">
       <c r="A236">
@@ -8062,7 +8069,7 @@
       <c r="B236" s="30">
         <v>7</v>
       </c>
-      <c r="C236" s="38"/>
+      <c r="C236" s="43"/>
     </row>
     <row r="237" spans="1:3">
       <c r="A237">
@@ -8071,7 +8078,7 @@
       <c r="B237" s="30">
         <v>8</v>
       </c>
-      <c r="C237" s="38"/>
+      <c r="C237" s="43"/>
     </row>
     <row r="238" spans="1:3">
       <c r="A238">
@@ -8080,7 +8087,7 @@
       <c r="B238" s="30">
         <v>9</v>
       </c>
-      <c r="C238" s="38"/>
+      <c r="C238" s="43"/>
     </row>
     <row r="239" spans="1:3">
       <c r="A239">
@@ -8089,7 +8096,7 @@
       <c r="B239" s="30">
         <v>10</v>
       </c>
-      <c r="C239" s="38"/>
+      <c r="C239" s="43"/>
     </row>
     <row r="240" spans="1:3">
       <c r="A240">
@@ -8098,7 +8105,7 @@
       <c r="B240" s="30">
         <v>11</v>
       </c>
-      <c r="C240" s="38"/>
+      <c r="C240" s="43"/>
     </row>
     <row r="241" spans="1:3">
       <c r="A241">
@@ -8107,7 +8114,7 @@
       <c r="B241" s="30">
         <v>12</v>
       </c>
-      <c r="C241" s="38"/>
+      <c r="C241" s="43"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242">
@@ -8116,7 +8123,7 @@
       <c r="B242" s="30">
         <v>13</v>
       </c>
-      <c r="C242" s="38"/>
+      <c r="C242" s="43"/>
     </row>
     <row r="243" spans="1:3">
       <c r="A243">
@@ -8125,7 +8132,7 @@
       <c r="B243" s="30">
         <v>14</v>
       </c>
-      <c r="C243" s="38"/>
+      <c r="C243" s="43"/>
     </row>
     <row r="244" spans="1:3">
       <c r="A244">
@@ -8134,7 +8141,7 @@
       <c r="B244" s="30">
         <v>15</v>
       </c>
-      <c r="C244" s="38"/>
+      <c r="C244" s="43"/>
     </row>
     <row r="245" spans="1:3">
       <c r="A245">
@@ -8143,7 +8150,7 @@
       <c r="B245" s="30">
         <v>16</v>
       </c>
-      <c r="C245" s="38"/>
+      <c r="C245" s="43"/>
     </row>
     <row r="246" spans="1:3">
       <c r="A246">
@@ -8152,7 +8159,7 @@
       <c r="B246" s="30">
         <v>17</v>
       </c>
-      <c r="C246" s="38"/>
+      <c r="C246" s="43"/>
     </row>
     <row r="247" spans="1:3">
       <c r="A247">
@@ -8161,7 +8168,7 @@
       <c r="B247" s="30">
         <v>18</v>
       </c>
-      <c r="C247" s="38"/>
+      <c r="C247" s="43"/>
     </row>
     <row r="248" spans="1:3">
       <c r="A248">
@@ -8170,7 +8177,7 @@
       <c r="B248" s="30">
         <v>19</v>
       </c>
-      <c r="C248" s="38"/>
+      <c r="C248" s="43"/>
     </row>
     <row r="249" spans="1:3">
       <c r="A249">
@@ -8179,7 +8186,7 @@
       <c r="B249" s="30">
         <v>20</v>
       </c>
-      <c r="C249" s="38"/>
+      <c r="C249" s="43"/>
     </row>
     <row r="250" spans="1:3">
       <c r="A250">
@@ -8188,7 +8195,7 @@
       <c r="B250" s="30">
         <v>21</v>
       </c>
-      <c r="C250" s="38"/>
+      <c r="C250" s="43"/>
     </row>
     <row r="251" spans="1:3">
       <c r="A251">
@@ -8197,7 +8204,7 @@
       <c r="B251" s="30">
         <v>22</v>
       </c>
-      <c r="C251" s="38"/>
+      <c r="C251" s="43"/>
     </row>
     <row r="252" spans="1:3">
       <c r="A252">
@@ -8206,7 +8213,7 @@
       <c r="B252" s="30">
         <v>23</v>
       </c>
-      <c r="C252" s="38"/>
+      <c r="C252" s="43"/>
     </row>
     <row r="253" spans="1:3">
       <c r="A253">
@@ -8215,7 +8222,7 @@
       <c r="B253" s="30">
         <v>24</v>
       </c>
-      <c r="C253" s="38"/>
+      <c r="C253" s="43"/>
     </row>
     <row r="254" spans="1:3">
       <c r="A254">
@@ -8224,7 +8231,7 @@
       <c r="B254" s="30">
         <v>25</v>
       </c>
-      <c r="C254" s="38"/>
+      <c r="C254" s="43"/>
     </row>
     <row r="255" spans="1:3">
       <c r="A255">
@@ -8233,7 +8240,7 @@
       <c r="B255" s="30">
         <v>26</v>
       </c>
-      <c r="C255" s="38"/>
+      <c r="C255" s="43"/>
     </row>
     <row r="256" spans="1:3">
       <c r="A256">
@@ -8242,7 +8249,7 @@
       <c r="B256" s="30">
         <v>27</v>
       </c>
-      <c r="C256" s="38"/>
+      <c r="C256" s="43"/>
     </row>
     <row r="257" spans="1:3">
       <c r="A257">
@@ -8251,7 +8258,7 @@
       <c r="B257" s="30">
         <v>28</v>
       </c>
-      <c r="C257" s="38"/>
+      <c r="C257" s="43"/>
     </row>
     <row r="258" spans="1:3">
       <c r="A258">
@@ -8260,7 +8267,7 @@
       <c r="B258" s="30">
         <v>29</v>
       </c>
-      <c r="C258" s="38"/>
+      <c r="C258" s="43"/>
     </row>
     <row r="259" spans="1:3">
       <c r="A259">
@@ -8269,7 +8276,7 @@
       <c r="B259" s="30">
         <v>30</v>
       </c>
-      <c r="C259" s="38"/>
+      <c r="C259" s="43"/>
     </row>
     <row r="260" spans="1:3">
       <c r="A260">
@@ -8278,7 +8285,7 @@
       <c r="B260" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C260" s="38"/>
+      <c r="C260" s="43"/>
     </row>
     <row r="261" spans="1:3" ht="15" thickBot="1">
       <c r="B261" s="2"/>
@@ -8286,7 +8293,7 @@
     </row>
     <row r="262" spans="1:3" ht="30">
       <c r="B262" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C262" s="15"/>
     </row>
@@ -8318,7 +8325,7 @@
     </row>
     <row r="266" spans="1:3" ht="30">
       <c r="B266" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C266" s="15"/>
     </row>
@@ -8372,7 +8379,7 @@
     </row>
     <row r="272" spans="1:3" ht="15">
       <c r="B272" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C272" s="15"/>
     </row>
@@ -8381,7 +8388,7 @@
         <v>1</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C273" s="15">
         <v>1</v>
@@ -8392,7 +8399,7 @@
         <v>2</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C274" s="15">
         <v>1</v>
@@ -8403,7 +8410,7 @@
         <v>3</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C275" s="15">
         <v>1</v>
@@ -8414,7 +8421,7 @@
         <v>4</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C276" s="15">
         <v>0.9</v>
@@ -8425,7 +8432,7 @@
         <v>5</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C277" s="15">
         <v>1</v>
@@ -8436,7 +8443,7 @@
         <v>6</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C278" s="15">
         <v>1</v>
@@ -8447,7 +8454,7 @@
         <v>7</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C279" s="15">
         <v>0.8</v>
@@ -8458,7 +8465,7 @@
         <v>8</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C280" s="15">
         <v>1</v>
@@ -8469,7 +8476,7 @@
         <v>9</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C281" s="15">
         <v>1</v>
@@ -8480,7 +8487,7 @@
         <v>10</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C282" s="15">
         <v>1</v>
@@ -8491,7 +8498,7 @@
         <v>11</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C283" s="15">
         <v>1</v>
@@ -8502,7 +8509,7 @@
         <v>12</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C284" s="15">
         <v>0.9</v>
@@ -8513,7 +8520,7 @@
         <v>13</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C285" s="15">
         <v>0.8</v>
@@ -8524,7 +8531,7 @@
         <v>14</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C286" s="15">
         <v>0.8</v>
@@ -8535,7 +8542,7 @@
         <v>15</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C287" s="15">
         <v>1</v>
@@ -8546,7 +8553,7 @@
         <v>16</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C288" s="15">
         <v>0.9</v>
@@ -8558,7 +8565,7 @@
     </row>
     <row r="290" spans="1:38" ht="15">
       <c r="B290" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C290" s="15"/>
     </row>
@@ -8573,7 +8580,7 @@
         <v>1</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C292" s="15">
         <v>1.8</v>
@@ -8584,7 +8591,7 @@
         <v>2</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C293" s="15">
         <v>1</v>
@@ -8595,7 +8602,7 @@
         <v>3</v>
       </c>
       <c r="B294" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C294" s="15">
         <v>0.7</v>
@@ -8656,7 +8663,7 @@
         <v>4</v>
       </c>
       <c r="B296" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C296" s="18">
         <v>0.6</v>
@@ -8693,7 +8700,7 @@
         <v>5</v>
       </c>
       <c r="B297" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C297" s="18">
         <v>0.75</v>
@@ -8730,7 +8737,7 @@
         <v>6</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C298" s="18">
         <v>0.4</v>
@@ -8767,7 +8774,7 @@
         <v>7</v>
       </c>
       <c r="B299" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C299" s="18">
         <v>0.8</v>
@@ -8804,7 +8811,7 @@
         <v>8</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C300" s="18">
         <v>0.28000000000000003</v>
@@ -8841,7 +8848,7 @@
         <v>9</v>
       </c>
       <c r="B301" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C301" s="18">
         <v>0.53</v>
@@ -8878,7 +8885,7 @@
         <v>10</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C302" s="18">
         <v>0.41</v>
@@ -8915,7 +8922,7 @@
         <v>11</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C303" s="18">
         <v>0.31</v>
@@ -8952,7 +8959,7 @@
         <v>12</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C304" s="18">
         <v>0.43</v>
@@ -8989,7 +8996,7 @@
         <v>13</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C305" s="18">
         <v>0.73</v>
@@ -9026,7 +9033,7 @@
         <v>14</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C306" s="18">
         <v>0.35</v>
@@ -9063,7 +9070,7 @@
         <v>15</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C307" s="18">
         <v>0.31</v>
@@ -9100,7 +9107,7 @@
         <v>16</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C308" s="18">
         <v>0.35</v>
@@ -9137,7 +9144,7 @@
         <v>17</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C309" s="18">
         <v>0.32</v>
@@ -9174,7 +9181,7 @@
         <v>18</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C310" s="18">
         <v>0.35</v>
@@ -9212,7 +9219,7 @@
     </row>
     <row r="312" spans="1:38" ht="15">
       <c r="B312" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C312" s="15"/>
     </row>
@@ -9255,7 +9262,7 @@
     </row>
     <row r="317" spans="1:38" ht="15">
       <c r="B317" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C317" s="15"/>
     </row>
@@ -10080,7 +10087,7 @@
         <v>124</v>
       </c>
       <c r="C361" s="21" t="s">
-        <v>126</v>
+        <v>239</v>
       </c>
     </row>
     <row r="362" spans="2:38" ht="15">
@@ -10088,7 +10095,7 @@
         <v>125</v>
       </c>
       <c r="C362" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="363" spans="2:38">
@@ -10177,7 +10184,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
[inspection, oversight calculators] constrain selection on the client side, refactor to use function composition
</commit_message>
<xml_diff>
--- a/public/local/fixtures/calculator/Обследование калькуляторы.xlsx
+++ b/public/local/fixtures/calculator/Обследование калькуляторы.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37580" windowHeight="21140" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37620" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Обследование одного здания" sheetId="3" r:id="rId1"/>
@@ -1364,7 +1364,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1408,6 +1408,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1543,7 +1547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="75">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1587,6 +1591,8 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1606,6 +1612,8 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1884,7 +1892,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1894,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D251" sqref="D251"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4468,7 +4476,7 @@
     </row>
     <row r="193" spans="1:32" s="16" customFormat="1">
       <c r="A193" s="38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B193" s="4" t="s">
         <v>183</v>
@@ -4511,7 +4519,7 @@
     </row>
     <row r="194" spans="1:32" s="16" customFormat="1" ht="46.5" customHeight="1">
       <c r="A194" s="38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B194" s="4" t="s">
         <v>184</v>
@@ -4554,7 +4562,7 @@
     </row>
     <row r="195" spans="1:32" s="16" customFormat="1" ht="46.5" customHeight="1">
       <c r="A195" s="38">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B195" s="4" t="s">
         <v>185</v>
@@ -4597,7 +4605,7 @@
     </row>
     <row r="196" spans="1:32" s="16" customFormat="1">
       <c r="A196" s="38">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>186</v>
@@ -4640,7 +4648,7 @@
     </row>
     <row r="197" spans="1:32" s="16" customFormat="1" ht="30.75" customHeight="1">
       <c r="A197" s="38">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B197" s="4" t="s">
         <v>187</v>
@@ -4683,7 +4691,7 @@
     </row>
     <row r="198" spans="1:32" s="16" customFormat="1" ht="30.75" customHeight="1">
       <c r="A198" s="38">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B198" s="4" t="s">
         <v>188</v>
@@ -4726,7 +4734,7 @@
     </row>
     <row r="199" spans="1:32" s="16" customFormat="1" ht="19.5" customHeight="1">
       <c r="A199" s="38">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B199" s="4" t="s">
         <v>189</v>
@@ -4769,7 +4777,7 @@
     </row>
     <row r="200" spans="1:32" s="16" customFormat="1" ht="18.75" customHeight="1">
       <c r="A200" s="38">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B200" s="4" t="s">
         <v>190</v>
@@ -4812,7 +4820,7 @@
     </row>
     <row r="201" spans="1:32" s="16" customFormat="1" ht="18.75" customHeight="1">
       <c r="A201" s="38">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B201" s="4" t="s">
         <v>191</v>
@@ -4855,7 +4863,7 @@
     </row>
     <row r="202" spans="1:32" s="16" customFormat="1" ht="18" customHeight="1">
       <c r="A202" s="38">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>192</v>
@@ -4898,7 +4906,7 @@
     </row>
     <row r="203" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1">
       <c r="A203" s="38">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B203" s="4" t="s">
         <v>193</v>
@@ -4941,7 +4949,7 @@
     </row>
     <row r="204" spans="1:32" s="16" customFormat="1" ht="15.75" customHeight="1">
       <c r="A204" s="38">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B204" s="4" t="s">
         <v>194</v>
@@ -4984,7 +4992,7 @@
     </row>
     <row r="205" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1">
       <c r="A205" s="38">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B205" s="4" t="s">
         <v>195</v>
@@ -5027,7 +5035,7 @@
     </row>
     <row r="206" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1">
       <c r="A206" s="38">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B206" s="4" t="s">
         <v>196</v>
@@ -5070,7 +5078,7 @@
     </row>
     <row r="207" spans="1:32" s="16" customFormat="1" ht="32.25" customHeight="1">
       <c r="A207" s="38">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>197</v>
@@ -5587,8 +5595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="D250" sqref="D250"/>
+    <sheetView topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="B294" sqref="B294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10241,6 +10249,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>